<commit_message>
Province Economy part 2 complete
</commit_message>
<xml_diff>
--- a/storage/provinces.xlsx
+++ b/storage/provinces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\laravel\wd_game\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C05258-C3FC-47AC-889F-B093EE520D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1A1BBC-10FA-46C6-809D-1B1B0F2BCEC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{F130E9F6-C185-4A85-AD65-7A53D08F0347}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>França</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Granada</t>
   </si>
   <si>
-    <t>Catalunia</t>
-  </si>
-  <si>
     <t>Douro</t>
   </si>
   <si>
@@ -129,7 +126,49 @@
     <t>Provence</t>
   </si>
   <si>
-    <t>Alsacia-Lorena</t>
+    <t>Catalonia</t>
+  </si>
+  <si>
+    <t>Alsace-Lorraine</t>
+  </si>
+  <si>
+    <t>Ulster</t>
+  </si>
+  <si>
+    <t>Leinster-Connacht</t>
+  </si>
+  <si>
+    <t>Munster</t>
+  </si>
+  <si>
+    <t>Highlands</t>
+  </si>
+  <si>
+    <t>Lowlands</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>North West England</t>
+  </si>
+  <si>
+    <t>North East England</t>
+  </si>
+  <si>
+    <t>Midlands</t>
+  </si>
+  <si>
+    <t>Eastern Counties</t>
+  </si>
+  <si>
+    <t>South East England</t>
+  </si>
+  <si>
+    <t>South West England</t>
+  </si>
+  <si>
+    <t>Reino Unido</t>
   </si>
 </sst>
 </file>
@@ -158,15 +197,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,15 +219,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BE9E85-215E-4FDB-9AF9-9674F5D52415}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,11 +579,11 @@
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -528,12 +595,21 @@
       <c r="E1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F1">
+        <v>10000</v>
+      </c>
+      <c r="G1">
+        <v>10000</v>
+      </c>
+      <c r="H1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -545,12 +621,21 @@
       <c r="E2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -562,12 +647,21 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F3">
+        <v>10000</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C4">
@@ -579,12 +673,21 @@
       <c r="E4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="F4">
+        <v>10000</v>
+      </c>
+      <c r="G4">
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C5">
@@ -596,12 +699,21 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="F5">
+        <v>10000</v>
+      </c>
+      <c r="G5">
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C6">
@@ -613,12 +725,21 @@
       <c r="E6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="F6">
+        <v>10000</v>
+      </c>
+      <c r="G6">
+        <v>10000</v>
+      </c>
+      <c r="H6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7">
@@ -630,12 +751,21 @@
       <c r="E7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="F7">
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <v>10000</v>
+      </c>
+      <c r="H7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C8">
@@ -647,12 +777,21 @@
       <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F8">
+        <v>10000</v>
+      </c>
+      <c r="G8">
+        <v>10000</v>
+      </c>
+      <c r="H8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C9">
@@ -664,12 +803,21 @@
       <c r="E9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="F9">
+        <v>10000</v>
+      </c>
+      <c r="G9">
+        <v>10000</v>
+      </c>
+      <c r="H9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C10">
@@ -681,12 +829,21 @@
       <c r="E10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="F10">
+        <v>10000</v>
+      </c>
+      <c r="G10">
+        <v>10000</v>
+      </c>
+      <c r="H10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C11">
@@ -698,12 +855,21 @@
       <c r="E11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="F11">
+        <v>10000</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C12">
@@ -715,12 +881,21 @@
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>10000</v>
+      </c>
+      <c r="G12">
+        <v>10000</v>
+      </c>
+      <c r="H12">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C13">
@@ -732,12 +907,21 @@
       <c r="E13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>10000</v>
+      </c>
+      <c r="G13">
+        <v>10000</v>
+      </c>
+      <c r="H13">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C14">
@@ -749,12 +933,21 @@
       <c r="E14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="F14">
+        <v>10000</v>
+      </c>
+      <c r="G14">
+        <v>10000</v>
+      </c>
+      <c r="H14">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C15">
@@ -766,12 +959,21 @@
       <c r="E15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="F15">
+        <v>10000</v>
+      </c>
+      <c r="G15">
+        <v>10000</v>
+      </c>
+      <c r="H15">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C16">
@@ -783,12 +985,21 @@
       <c r="E16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="F16">
+        <v>10000</v>
+      </c>
+      <c r="G16">
+        <v>10000</v>
+      </c>
+      <c r="H16">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C17">
@@ -800,12 +1011,21 @@
       <c r="E17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="F17">
+        <v>10000</v>
+      </c>
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C18">
@@ -817,46 +1037,73 @@
       <c r="E18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>10000</v>
+      </c>
+      <c r="G18">
+        <v>10000</v>
+      </c>
+      <c r="H18">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>10000</v>
+      </c>
+      <c r="G19">
+        <v>10000</v>
+      </c>
+      <c r="H19">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>10000</v>
+      </c>
+      <c r="G20">
+        <v>10000</v>
+      </c>
+      <c r="H20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C21">
@@ -868,12 +1115,21 @@
       <c r="E21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>10000</v>
+      </c>
+      <c r="G21">
+        <v>10000</v>
+      </c>
+      <c r="H21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C22">
@@ -885,12 +1141,21 @@
       <c r="E22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>10000</v>
+      </c>
+      <c r="G22">
+        <v>10000</v>
+      </c>
+      <c r="H22">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C23">
@@ -902,12 +1167,21 @@
       <c r="E23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>10000</v>
+      </c>
+      <c r="G23">
+        <v>10000</v>
+      </c>
+      <c r="H23">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C24">
@@ -919,12 +1193,21 @@
       <c r="E24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>10000</v>
+      </c>
+      <c r="G24">
+        <v>10000</v>
+      </c>
+      <c r="H24">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C25">
@@ -936,12 +1219,21 @@
       <c r="E25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>10000</v>
+      </c>
+      <c r="G25">
+        <v>10000</v>
+      </c>
+      <c r="H25">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C26">
@@ -953,12 +1245,21 @@
       <c r="E26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F26">
+        <v>10000</v>
+      </c>
+      <c r="G26">
+        <v>10000</v>
+      </c>
+      <c r="H26">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C27">
@@ -970,12 +1271,21 @@
       <c r="E27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="F27">
+        <v>10000</v>
+      </c>
+      <c r="G27">
+        <v>10000</v>
+      </c>
+      <c r="H27">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C28">
@@ -987,12 +1297,21 @@
       <c r="E28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="F28">
+        <v>10000</v>
+      </c>
+      <c r="G28">
+        <v>10000</v>
+      </c>
+      <c r="H28">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C29">
@@ -1004,12 +1323,21 @@
       <c r="E29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="F29">
+        <v>10000</v>
+      </c>
+      <c r="G29">
+        <v>10000</v>
+      </c>
+      <c r="H29">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C30">
@@ -1021,6 +1349,359 @@
       <c r="E30">
         <v>4</v>
       </c>
+      <c r="F30">
+        <v>10000</v>
+      </c>
+      <c r="G30">
+        <v>10000</v>
+      </c>
+      <c r="H30">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>10000</v>
+      </c>
+      <c r="G31">
+        <v>10000</v>
+      </c>
+      <c r="H31">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>10000</v>
+      </c>
+      <c r="G32">
+        <v>10000</v>
+      </c>
+      <c r="H32">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>10000</v>
+      </c>
+      <c r="G33">
+        <v>10000</v>
+      </c>
+      <c r="H33">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>10000</v>
+      </c>
+      <c r="G34">
+        <v>10000</v>
+      </c>
+      <c r="H34">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>10000</v>
+      </c>
+      <c r="G35">
+        <v>10000</v>
+      </c>
+      <c r="H35">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>10000</v>
+      </c>
+      <c r="G36">
+        <v>10000</v>
+      </c>
+      <c r="H36">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>10000</v>
+      </c>
+      <c r="G37">
+        <v>10000</v>
+      </c>
+      <c r="H37">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>10000</v>
+      </c>
+      <c r="G38">
+        <v>10000</v>
+      </c>
+      <c r="H38">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>10000</v>
+      </c>
+      <c r="G39">
+        <v>10000</v>
+      </c>
+      <c r="H39">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>10000</v>
+      </c>
+      <c r="G40">
+        <v>10000</v>
+      </c>
+      <c r="H40">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>10000</v>
+      </c>
+      <c r="G41">
+        <v>10000</v>
+      </c>
+      <c r="H41">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>10000</v>
+      </c>
+      <c r="G42">
+        <v>10000</v>
+      </c>
+      <c r="H42">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>10000</v>
+      </c>
+      <c r="G43">
+        <v>10000</v>
+      </c>
+      <c r="H43">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>